<commit_message>
added merged_data_modified.csv to /static/data main folder
</commit_message>
<xml_diff>
--- a/Kip/ColumnLoss.xlsx
+++ b/Kip/ColumnLoss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kip Madden\Desktop\dataScience\project-2\Kip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D8AFDB-1E03-411D-9C17-43A6E8886EAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D725B26B-0363-4AC1-9BB1-D55E77101214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="10" xr2:uid="{526A8007-2B7C-4A99-9DA7-25FE95362C64}"/>
+    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="9" xr2:uid="{526A8007-2B7C-4A99-9DA7-25FE95362C64}"/>
   </bookViews>
   <sheets>
     <sheet name="six" sheetId="1" r:id="rId1"/>
@@ -1722,27 +1722,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -5524,8 +5508,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794F44C-EF74-4DB1-A296-7454105E884B}">
   <dimension ref="A1:I221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B178" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A94" sqref="A94:I221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -11285,7 +11272,7 @@
   </sheetData>
   <autoFilter ref="A1:I221" xr:uid="{DEA5BD02-8103-4309-86C3-AC14A76234C0}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I221">
-      <sortCondition sortBy="cellColor" ref="B1:B221" dxfId="3"/>
+      <sortCondition sortBy="cellColor" ref="B1:B221" dxfId="1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11296,8 +11283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38E6739-9B40-44D2-8E43-EE8588420DA3}">
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -12289,7 +12276,7 @@
   </sheetData>
   <autoFilter ref="A1:H93" xr:uid="{C12001EC-F0F9-4691-B73C-C5C9ACF58417}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H93">
-      <sortCondition sortBy="cellColor" ref="B1:B93" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="B1:B93" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15545,7 +15532,7 @@
   <dimension ref="A1:I221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>

</xml_diff>